<commit_message>
Capitalization of column headings in tables
</commit_message>
<xml_diff>
--- a/hybrid_searchTesting/timings_avarage_20_40_60_questions_DBFS.xlsx
+++ b/hybrid_searchTesting/timings_avarage_20_40_60_questions_DBFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\hybrid_searchTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC5FD68-CAEB-42BD-B1D9-A111387745EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9249D05-7AB9-47B7-A640-59DC9890C63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{606D70C8-7B5B-495A-B68E-FE4388FD4562}"/>
   </bookViews>
@@ -38,33 +38,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
-    <t>kérdések száma</t>
-  </si>
-  <si>
-    <t>embedding  generálásai idő átlaga</t>
-  </si>
-  <si>
-    <t>sparse embedding generálási idő átlaga</t>
-  </si>
-  <si>
-    <t>kontextus összeállitási idő átlaga</t>
-  </si>
-  <si>
     <t>LLM feldolgozási idő átlaga</t>
   </si>
   <si>
-    <t>teljes feldoldozási idő átlaga</t>
-  </si>
-  <si>
-    <t>szemantikus hasonlóság mérékének  (BERTScore F1) átlaga (0-1) között</t>
-  </si>
-  <si>
-    <t>top_k darab számának átlag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LLM modell: gemini-2.0-flash; </t>
-  </si>
-  <si>
     <t>0.59/s</t>
   </si>
   <si>
@@ -102,6 +78,30 @@
   </si>
   <si>
     <t>5.63/s</t>
+  </si>
+  <si>
+    <t>Kérdések száma</t>
+  </si>
+  <si>
+    <t>Embedding  generálásai idő átlaga</t>
+  </si>
+  <si>
+    <t>Kontextus összeállitási idő átlaga</t>
+  </si>
+  <si>
+    <t>Teljes feldoldozási idő átlaga</t>
+  </si>
+  <si>
+    <t>Szemantikus hasonlóság mérékének  (BERTScore F1) átlaga (0-1) között</t>
+  </si>
+  <si>
+    <t>Top_k darab számának átlag</t>
+  </si>
+  <si>
+    <t>Sparse embedding generálási idő átlaga</t>
+  </si>
+  <si>
+    <t>LLM modell: gemini-2.0-flash;  DBFS</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
   <dimension ref="B2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,7 +592,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -604,28 +604,28 @@
     </row>
     <row r="3" spans="2:9" ht="78" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -633,19 +633,19 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1">
         <v>0.87</v>
@@ -659,19 +659,19 @@
         <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H5" s="1">
         <v>0.84</v>
@@ -685,19 +685,19 @@
         <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1">
         <v>0.85</v>

</xml_diff>